<commit_message>
CIS variables, vocabulary update
</commit_message>
<xml_diff>
--- a/DMP/docs/Appendix_I_ACTRIS-RI_variables_4May2023.xlsx
+++ b/DMP/docs/Appendix_I_ACTRIS-RI_variables_4May2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clm\Work Folders\NILU\forskning\projects\ACTRIS-PPP\WP4\DC_concept\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F2FCD625-88F2-48B3-A6C2-8D1849F8A3FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BCE4A3C3-AC67-4500-8EF4-186F613DF214}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="75" yWindow="0" windowWidth="25935" windowHeight="17385" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="75" yWindow="0" windowWidth="25935" windowHeight="17385" firstSheet="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ACTRIS RI Variables" sheetId="12" r:id="rId1"/>
@@ -714,7 +714,7 @@
     </r>
   </si>
   <si>
-    <t>Liquid Water Content</t>
+    <t>Liquid droplet mass concentration</t>
   </si>
   <si>
     <t>only during cloud periods</t>
@@ -729,13 +729,13 @@
     <t>1 min</t>
   </si>
   <si>
-    <t>Droplet effective radius</t>
-  </si>
-  <si>
-    <t>Droplet number concentration</t>
-  </si>
-  <si>
-    <t>Droplet size distribution</t>
+    <t>Liquid droplet effective radius</t>
+  </si>
+  <si>
+    <t>Liquid droplet number concentration</t>
+  </si>
+  <si>
+    <t>Liquid droplet number size distribution</t>
   </si>
   <si>
     <t>Ice particle number concentration</t>
@@ -744,7 +744,7 @@
     <t>only during mixed-phase cloud periods</t>
   </si>
   <si>
-    <t>Ice particle size distribution</t>
+    <t>Ice particle number size distribution</t>
   </si>
   <si>
     <t>Ice nucleating particle number concentration</t>
@@ -2725,6 +2725,30 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="32" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="33" fillId="12" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="33" fillId="13" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="14" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="27" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="27" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2767,9 +2791,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2779,35 +2800,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="32" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="33" fillId="12" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="33" fillId="13" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="14" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="14" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="14" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="27" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="27" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="33" fillId="12" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -6318,9 +6318,9 @@
   </sheetPr>
   <dimension ref="A1:BK79"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="7" topLeftCell="B55" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="A67" sqref="A67"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane xSplit="1" ySplit="7" topLeftCell="B67" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="A79" sqref="A68:A79"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
     </sheetView>
@@ -6372,15 +6372,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62" ht="24" customHeight="1" thickBot="1">
-      <c r="A1" s="129" t="s">
+      <c r="A1" s="141" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="130" t="s">
+      <c r="B1" s="142" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="131"/>
-      <c r="D1" s="131"/>
-      <c r="E1" s="131"/>
+      <c r="C1" s="143"/>
+      <c r="D1" s="143"/>
+      <c r="E1" s="143"/>
       <c r="F1" s="71"/>
       <c r="G1" s="71"/>
       <c r="H1" s="71"/>
@@ -6394,16 +6394,16 @@
       <c r="P1" s="75"/>
     </row>
     <row r="2" spans="1:62" ht="14.1" customHeight="1">
-      <c r="A2" s="129"/>
-      <c r="B2" s="132" t="s">
+      <c r="A2" s="141"/>
+      <c r="B2" s="144" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="133"/>
-      <c r="D2" s="133"/>
-      <c r="E2" s="133"/>
-      <c r="F2" s="133"/>
-      <c r="G2" s="133"/>
-      <c r="H2" s="133"/>
+      <c r="C2" s="145"/>
+      <c r="D2" s="145"/>
+      <c r="E2" s="145"/>
+      <c r="F2" s="145"/>
+      <c r="G2" s="145"/>
+      <c r="H2" s="145"/>
       <c r="I2" s="9"/>
       <c r="J2" s="9"/>
       <c r="K2" s="9"/>
@@ -6416,18 +6416,18 @@
       <c r="AT2" s="7"/>
     </row>
     <row r="3" spans="1:62" ht="15" customHeight="1">
-      <c r="A3" s="129"/>
-      <c r="B3" s="140" t="s">
+      <c r="A3" s="141"/>
+      <c r="B3" s="152" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="141"/>
-      <c r="D3" s="141"/>
-      <c r="E3" s="142"/>
-      <c r="F3" s="142"/>
-      <c r="G3" s="142"/>
-      <c r="H3" s="141"/>
-      <c r="I3" s="141"/>
-      <c r="J3" s="141"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="154"/>
+      <c r="F3" s="154"/>
+      <c r="G3" s="154"/>
+      <c r="H3" s="153"/>
+      <c r="I3" s="153"/>
+      <c r="J3" s="153"/>
       <c r="K3" s="77"/>
       <c r="L3" s="77"/>
       <c r="M3" s="28">
@@ -6439,18 +6439,18 @@
       <c r="AW3" s="1"/>
     </row>
     <row r="4" spans="1:62" ht="15.75" thickBot="1">
-      <c r="A4" s="129"/>
-      <c r="B4" s="134" t="s">
+      <c r="A4" s="141"/>
+      <c r="B4" s="146" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="135"/>
-      <c r="D4" s="135"/>
-      <c r="E4" s="136"/>
-      <c r="F4" s="136"/>
-      <c r="G4" s="136"/>
-      <c r="H4" s="135"/>
-      <c r="I4" s="135"/>
-      <c r="J4" s="135"/>
+      <c r="C4" s="147"/>
+      <c r="D4" s="147"/>
+      <c r="E4" s="148"/>
+      <c r="F4" s="148"/>
+      <c r="G4" s="148"/>
+      <c r="H4" s="147"/>
+      <c r="I4" s="147"/>
+      <c r="J4" s="147"/>
       <c r="K4" s="18"/>
       <c r="L4" s="18"/>
       <c r="M4" s="29">
@@ -6477,53 +6477,53 @@
       <c r="M6" s="80"/>
       <c r="N6" s="79"/>
       <c r="O6" s="79"/>
-      <c r="P6" s="138" t="s">
+      <c r="P6" s="150" t="s">
         <v>5</v>
       </c>
-      <c r="Q6" s="137"/>
-      <c r="R6" s="137"/>
-      <c r="S6" s="138"/>
-      <c r="T6" s="137"/>
-      <c r="U6" s="137"/>
-      <c r="V6" s="137"/>
-      <c r="W6" s="137"/>
-      <c r="X6" s="137"/>
-      <c r="Y6" s="137"/>
-      <c r="Z6" s="137"/>
-      <c r="AA6" s="137"/>
-      <c r="AB6" s="137"/>
-      <c r="AC6" s="137"/>
-      <c r="AD6" s="137"/>
-      <c r="AE6" s="137"/>
-      <c r="AF6" s="137" t="s">
+      <c r="Q6" s="149"/>
+      <c r="R6" s="149"/>
+      <c r="S6" s="150"/>
+      <c r="T6" s="149"/>
+      <c r="U6" s="149"/>
+      <c r="V6" s="149"/>
+      <c r="W6" s="149"/>
+      <c r="X6" s="149"/>
+      <c r="Y6" s="149"/>
+      <c r="Z6" s="149"/>
+      <c r="AA6" s="149"/>
+      <c r="AB6" s="149"/>
+      <c r="AC6" s="149"/>
+      <c r="AD6" s="149"/>
+      <c r="AE6" s="149"/>
+      <c r="AF6" s="149" t="s">
         <v>5</v>
       </c>
-      <c r="AG6" s="139"/>
-      <c r="AH6" s="139"/>
-      <c r="AI6" s="139"/>
-      <c r="AJ6" s="139"/>
-      <c r="AK6" s="139"/>
-      <c r="AL6" s="139"/>
-      <c r="AM6" s="139"/>
-      <c r="AN6" s="139"/>
-      <c r="AO6" s="139"/>
-      <c r="AP6" s="139"/>
-      <c r="AQ6" s="139"/>
-      <c r="AR6" s="139"/>
-      <c r="AS6" s="139"/>
-      <c r="AT6" s="139"/>
-      <c r="AU6" s="139"/>
+      <c r="AG6" s="151"/>
+      <c r="AH6" s="151"/>
+      <c r="AI6" s="151"/>
+      <c r="AJ6" s="151"/>
+      <c r="AK6" s="151"/>
+      <c r="AL6" s="151"/>
+      <c r="AM6" s="151"/>
+      <c r="AN6" s="151"/>
+      <c r="AO6" s="151"/>
+      <c r="AP6" s="151"/>
+      <c r="AQ6" s="151"/>
+      <c r="AR6" s="151"/>
+      <c r="AS6" s="151"/>
+      <c r="AT6" s="151"/>
+      <c r="AU6" s="151"/>
       <c r="AV6" s="81"/>
-      <c r="AW6" s="137" t="s">
+      <c r="AW6" s="149" t="s">
         <v>5</v>
       </c>
-      <c r="AX6" s="137"/>
-      <c r="AY6" s="137"/>
-      <c r="AZ6" s="137"/>
-      <c r="BA6" s="137"/>
-      <c r="BB6" s="137"/>
-      <c r="BC6" s="137"/>
-      <c r="BD6" s="137"/>
+      <c r="AX6" s="149"/>
+      <c r="AY6" s="149"/>
+      <c r="AZ6" s="149"/>
+      <c r="BA6" s="149"/>
+      <c r="BB6" s="149"/>
+      <c r="BC6" s="149"/>
+      <c r="BD6" s="149"/>
       <c r="BE6" s="70"/>
       <c r="BF6" s="70"/>
       <c r="BG6" s="70"/>
@@ -9538,7 +9538,7 @@
       <c r="B39" s="106" t="s">
         <v>149</v>
       </c>
-      <c r="C39" s="143" t="s">
+      <c r="C39" s="140" t="s">
         <v>150</v>
       </c>
       <c r="D39" s="96">
@@ -9556,7 +9556,7 @@
       <c r="H39" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="I39" s="143" t="s">
+      <c r="I39" s="140" t="s">
         <v>150</v>
       </c>
       <c r="J39" s="5" t="s">
@@ -9636,7 +9636,7 @@
       <c r="B40" s="106" t="s">
         <v>155</v>
       </c>
-      <c r="C40" s="143"/>
+      <c r="C40" s="140"/>
       <c r="D40" s="96">
         <v>2</v>
       </c>
@@ -9652,7 +9652,7 @@
       <c r="H40" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="I40" s="143"/>
+      <c r="I40" s="140"/>
       <c r="J40" s="5" t="s">
         <v>101</v>
       </c>
@@ -9732,7 +9732,7 @@
       <c r="B41" s="106" t="s">
         <v>158</v>
       </c>
-      <c r="C41" s="143"/>
+      <c r="C41" s="140"/>
       <c r="D41" s="96">
         <v>2</v>
       </c>
@@ -9748,7 +9748,7 @@
       <c r="H41" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="I41" s="143"/>
+      <c r="I41" s="140"/>
       <c r="J41" s="5" t="s">
         <v>101</v>
       </c>
@@ -9828,7 +9828,7 @@
       <c r="B42" s="106" t="s">
         <v>160</v>
       </c>
-      <c r="C42" s="143"/>
+      <c r="C42" s="140"/>
       <c r="D42" s="96">
         <v>2</v>
       </c>
@@ -9844,7 +9844,7 @@
       <c r="H42" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="I42" s="143"/>
+      <c r="I42" s="140"/>
       <c r="J42" s="5" t="s">
         <v>101</v>
       </c>
@@ -9922,7 +9922,7 @@
       <c r="B43" s="106" t="s">
         <v>162</v>
       </c>
-      <c r="C43" s="143"/>
+      <c r="C43" s="140"/>
       <c r="D43" s="96">
         <v>2</v>
       </c>
@@ -9938,7 +9938,7 @@
       <c r="H43" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="I43" s="143"/>
+      <c r="I43" s="140"/>
       <c r="J43" s="5" t="s">
         <v>101</v>
       </c>
@@ -10020,7 +10020,7 @@
       <c r="B44" s="106" t="s">
         <v>160</v>
       </c>
-      <c r="C44" s="143"/>
+      <c r="C44" s="140"/>
       <c r="D44" s="96">
         <v>2</v>
       </c>
@@ -10036,7 +10036,7 @@
       <c r="H44" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="I44" s="143"/>
+      <c r="I44" s="140"/>
       <c r="J44" s="5" t="s">
         <v>101</v>
       </c>
@@ -10114,7 +10114,7 @@
       <c r="B45" s="106" t="s">
         <v>165</v>
       </c>
-      <c r="C45" s="143"/>
+      <c r="C45" s="140"/>
       <c r="D45" s="96">
         <v>2</v>
       </c>
@@ -10130,7 +10130,7 @@
       <c r="H45" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="I45" s="143"/>
+      <c r="I45" s="140"/>
       <c r="J45" s="5" t="s">
         <v>101</v>
       </c>
@@ -10208,7 +10208,7 @@
       <c r="B46" s="106" t="s">
         <v>165</v>
       </c>
-      <c r="C46" s="143"/>
+      <c r="C46" s="140"/>
       <c r="D46" s="96">
         <v>2</v>
       </c>
@@ -10224,7 +10224,7 @@
       <c r="H46" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="I46" s="143"/>
+      <c r="I46" s="140"/>
       <c r="J46" s="5" t="s">
         <v>101</v>
       </c>
@@ -10302,7 +10302,7 @@
       <c r="B47" s="106" t="s">
         <v>160</v>
       </c>
-      <c r="C47" s="143"/>
+      <c r="C47" s="140"/>
       <c r="D47" s="96">
         <v>2</v>
       </c>
@@ -10318,7 +10318,7 @@
       <c r="H47" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="I47" s="143"/>
+      <c r="I47" s="140"/>
       <c r="J47" s="5" t="s">
         <v>101</v>
       </c>
@@ -10396,7 +10396,7 @@
       <c r="B48" s="106" t="s">
         <v>160</v>
       </c>
-      <c r="C48" s="143"/>
+      <c r="C48" s="140"/>
       <c r="D48" s="96">
         <v>2</v>
       </c>
@@ -10412,7 +10412,7 @@
       <c r="H48" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="I48" s="143"/>
+      <c r="I48" s="140"/>
       <c r="J48" s="5" t="s">
         <v>101</v>
       </c>
@@ -12271,7 +12271,7 @@
       <c r="BK67" s="47"/>
     </row>
     <row r="68" spans="1:63">
-      <c r="A68" s="3" t="s">
+      <c r="A68" s="160" t="s">
         <v>208</v>
       </c>
       <c r="B68" s="21" t="s">
@@ -12368,7 +12368,7 @@
       <c r="BK68" s="5"/>
     </row>
     <row r="69" spans="1:63">
-      <c r="A69" s="3" t="s">
+      <c r="A69" s="40" t="s">
         <v>213</v>
       </c>
       <c r="B69" s="21" t="s">
@@ -12462,7 +12462,7 @@
       <c r="BK69" s="5"/>
     </row>
     <row r="70" spans="1:63">
-      <c r="A70" s="11" t="s">
+      <c r="A70" s="160" t="s">
         <v>214</v>
       </c>
       <c r="B70" s="21" t="s">
@@ -12559,7 +12559,7 @@
       <c r="BK70" s="5"/>
     </row>
     <row r="71" spans="1:63">
-      <c r="A71" s="11" t="s">
+      <c r="A71" s="21" t="s">
         <v>215</v>
       </c>
       <c r="B71" s="21" t="s">
@@ -12656,7 +12656,7 @@
       <c r="BK71" s="5"/>
     </row>
     <row r="72" spans="1:63">
-      <c r="A72" s="11" t="s">
+      <c r="A72" s="40" t="s">
         <v>216</v>
       </c>
       <c r="B72" s="21" t="s">
@@ -12753,7 +12753,7 @@
       <c r="BK72" s="5"/>
     </row>
     <row r="73" spans="1:63">
-      <c r="A73" s="11" t="s">
+      <c r="A73" s="160" t="s">
         <v>218</v>
       </c>
       <c r="B73" s="21" t="s">
@@ -12850,7 +12850,7 @@
       <c r="BK73" s="5"/>
     </row>
     <row r="74" spans="1:63">
-      <c r="A74" s="11" t="s">
+      <c r="A74" s="40" t="s">
         <v>219</v>
       </c>
       <c r="B74" s="21" t="s">
@@ -12947,7 +12947,7 @@
       <c r="BK74" s="5"/>
     </row>
     <row r="75" spans="1:63">
-      <c r="A75" s="11" t="s">
+      <c r="A75" s="40" t="s">
         <v>222</v>
       </c>
       <c r="B75" s="21" t="s">
@@ -13056,7 +13056,7 @@
       <c r="D76" s="4">
         <v>2</v>
       </c>
-      <c r="E76" s="148" t="s">
+      <c r="E76" s="4" t="s">
         <v>119</v>
       </c>
       <c r="F76" s="5" t="s">
@@ -13149,7 +13149,7 @@
       <c r="D77" s="4">
         <v>2</v>
       </c>
-      <c r="E77" s="148" t="s">
+      <c r="E77" s="4" t="s">
         <v>119</v>
       </c>
       <c r="F77" s="5" t="s">
@@ -13242,7 +13242,7 @@
       <c r="D78" s="4">
         <v>2</v>
       </c>
-      <c r="E78" s="149" t="s">
+      <c r="E78" s="130" t="s">
         <v>119</v>
       </c>
       <c r="F78" s="5" t="s">
@@ -13323,21 +13323,22 @@
       <c r="BJ78" s="91"/>
     </row>
     <row r="79" spans="1:63">
+      <c r="A79" s="40"/>
       <c r="Q79" s="50"/>
     </row>
   </sheetData>
   <autoFilter ref="A7:BJ75" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="10">
+    <mergeCell ref="AW6:BD6"/>
+    <mergeCell ref="P6:AE6"/>
+    <mergeCell ref="AF6:AU6"/>
+    <mergeCell ref="B3:J3"/>
     <mergeCell ref="I39:I48"/>
     <mergeCell ref="C39:C48"/>
     <mergeCell ref="A1:A4"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="B4:J4"/>
-    <mergeCell ref="AW6:BD6"/>
-    <mergeCell ref="P6:AE6"/>
-    <mergeCell ref="AF6:AU6"/>
-    <mergeCell ref="B3:J3"/>
   </mergeCells>
   <conditionalFormatting sqref="Q12:R16 Q11 Q18:R18 Q17 R19 Q20 AE35:AH36">
     <cfRule type="cellIs" dxfId="311" priority="1013" operator="equal">
@@ -14794,7 +14795,7 @@
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="144" t="s">
+      <c r="A4" s="155" t="s">
         <v>264</v>
       </c>
       <c r="B4" s="119" t="s">
@@ -15232,7 +15233,7 @@
       <c r="E41" s="125"/>
     </row>
     <row r="42" spans="1:5">
-      <c r="A42" s="144" t="s">
+      <c r="A42" s="155" t="s">
         <v>335</v>
       </c>
       <c r="B42" s="119" t="s">
@@ -15442,7 +15443,7 @@
       <c r="E59" s="125"/>
     </row>
     <row r="60" spans="1:5">
-      <c r="A60" s="144" t="s">
+      <c r="A60" s="155" t="s">
         <v>365</v>
       </c>
       <c r="B60" s="119" t="s">
@@ -15457,7 +15458,7 @@
       </c>
     </row>
     <row r="61" spans="1:5">
-      <c r="A61" s="145"/>
+      <c r="A61" s="156"/>
       <c r="B61" s="126" t="s">
         <v>368</v>
       </c>
@@ -15468,7 +15469,7 @@
       <c r="E61" s="122"/>
     </row>
     <row r="62" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A62" s="146"/>
+      <c r="A62" s="157"/>
       <c r="B62" s="127" t="s">
         <v>370</v>
       </c>
@@ -15488,7 +15489,7 @@
       <c r="E63" s="125"/>
     </row>
     <row r="64" spans="1:5">
-      <c r="A64" s="144" t="s">
+      <c r="A64" s="155" t="s">
         <v>371</v>
       </c>
       <c r="B64" s="119" t="s">
@@ -15503,7 +15504,7 @@
       </c>
     </row>
     <row r="65" spans="1:5">
-      <c r="A65" s="145"/>
+      <c r="A65" s="156"/>
       <c r="B65" s="121" t="s">
         <v>374</v>
       </c>
@@ -15516,7 +15517,7 @@
       </c>
     </row>
     <row r="66" spans="1:5">
-      <c r="A66" s="145"/>
+      <c r="A66" s="156"/>
       <c r="B66" s="121" t="s">
         <v>376</v>
       </c>
@@ -15527,7 +15528,7 @@
       <c r="E66" s="122"/>
     </row>
     <row r="67" spans="1:5">
-      <c r="A67" s="145"/>
+      <c r="A67" s="156"/>
       <c r="B67" s="121" t="s">
         <v>377</v>
       </c>
@@ -15538,7 +15539,7 @@
       <c r="E67" s="122"/>
     </row>
     <row r="68" spans="1:5">
-      <c r="A68" s="145"/>
+      <c r="A68" s="156"/>
       <c r="B68" s="121" t="s">
         <v>379</v>
       </c>
@@ -15549,7 +15550,7 @@
       <c r="E68" s="122"/>
     </row>
     <row r="69" spans="1:5">
-      <c r="A69" s="145"/>
+      <c r="A69" s="156"/>
       <c r="B69" s="121" t="s">
         <v>380</v>
       </c>
@@ -15562,7 +15563,7 @@
       </c>
     </row>
     <row r="70" spans="1:5">
-      <c r="A70" s="145"/>
+      <c r="A70" s="156"/>
       <c r="B70" s="121" t="s">
         <v>383</v>
       </c>
@@ -15575,7 +15576,7 @@
       </c>
     </row>
     <row r="71" spans="1:5">
-      <c r="A71" s="145"/>
+      <c r="A71" s="156"/>
       <c r="B71" s="121" t="s">
         <v>385</v>
       </c>
@@ -15588,7 +15589,7 @@
       </c>
     </row>
     <row r="72" spans="1:5">
-      <c r="A72" s="145"/>
+      <c r="A72" s="156"/>
       <c r="B72" s="121" t="s">
         <v>387</v>
       </c>
@@ -15599,7 +15600,7 @@
       <c r="E72" s="122"/>
     </row>
     <row r="73" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A73" s="146"/>
+      <c r="A73" s="157"/>
       <c r="B73" s="121" t="s">
         <v>389</v>
       </c>
@@ -15617,7 +15618,7 @@
       <c r="E74" s="125"/>
     </row>
     <row r="75" spans="1:5">
-      <c r="A75" s="144" t="s">
+      <c r="A75" s="155" t="s">
         <v>176</v>
       </c>
       <c r="B75" s="121" t="s">
@@ -15632,7 +15633,7 @@
       </c>
     </row>
     <row r="76" spans="1:5">
-      <c r="A76" s="145"/>
+      <c r="A76" s="156"/>
       <c r="B76" s="121" t="s">
         <v>393</v>
       </c>
@@ -15643,7 +15644,7 @@
       <c r="E76" s="122"/>
     </row>
     <row r="77" spans="1:5">
-      <c r="A77" s="145"/>
+      <c r="A77" s="156"/>
       <c r="B77" s="121" t="s">
         <v>394</v>
       </c>
@@ -15654,7 +15655,7 @@
       <c r="E77" s="122"/>
     </row>
     <row r="78" spans="1:5">
-      <c r="A78" s="145"/>
+      <c r="A78" s="156"/>
       <c r="B78" s="121" t="s">
         <v>396</v>
       </c>
@@ -15665,7 +15666,7 @@
       <c r="E78" s="122"/>
     </row>
     <row r="79" spans="1:5">
-      <c r="A79" s="145"/>
+      <c r="A79" s="156"/>
       <c r="B79" s="121" t="s">
         <v>398</v>
       </c>
@@ -15676,7 +15677,7 @@
       <c r="E79" s="122"/>
     </row>
     <row r="80" spans="1:5">
-      <c r="A80" s="145"/>
+      <c r="A80" s="156"/>
       <c r="B80" s="121" t="s">
         <v>400</v>
       </c>
@@ -15687,7 +15688,7 @@
       <c r="E80" s="122"/>
     </row>
     <row r="81" spans="1:5">
-      <c r="A81" s="145"/>
+      <c r="A81" s="156"/>
       <c r="B81" s="121" t="s">
         <v>402</v>
       </c>
@@ -15698,7 +15699,7 @@
       <c r="E81" s="122"/>
     </row>
     <row r="82" spans="1:5">
-      <c r="A82" s="145"/>
+      <c r="A82" s="156"/>
       <c r="B82" s="121" t="s">
         <v>403</v>
       </c>
@@ -15709,7 +15710,7 @@
       <c r="E82" s="122"/>
     </row>
     <row r="83" spans="1:5">
-      <c r="A83" s="145"/>
+      <c r="A83" s="156"/>
       <c r="B83" s="121" t="s">
         <v>404</v>
       </c>
@@ -15720,7 +15721,7 @@
       <c r="E83" s="122"/>
     </row>
     <row r="84" spans="1:5">
-      <c r="A84" s="145"/>
+      <c r="A84" s="156"/>
       <c r="B84" s="121" t="s">
         <v>406</v>
       </c>
@@ -15731,7 +15732,7 @@
       <c r="E84" s="122"/>
     </row>
     <row r="85" spans="1:5">
-      <c r="A85" s="145"/>
+      <c r="A85" s="156"/>
       <c r="B85" s="121" t="s">
         <v>408</v>
       </c>
@@ -15744,7 +15745,7 @@
       </c>
     </row>
     <row r="86" spans="1:5">
-      <c r="A86" s="145"/>
+      <c r="A86" s="156"/>
       <c r="B86" s="121" t="s">
         <v>410</v>
       </c>
@@ -15755,7 +15756,7 @@
       <c r="E86" s="122"/>
     </row>
     <row r="87" spans="1:5">
-      <c r="A87" s="145"/>
+      <c r="A87" s="156"/>
       <c r="B87" s="121" t="s">
         <v>411</v>
       </c>
@@ -15766,7 +15767,7 @@
       <c r="E87" s="122"/>
     </row>
     <row r="88" spans="1:5">
-      <c r="A88" s="145"/>
+      <c r="A88" s="156"/>
       <c r="B88" s="121" t="s">
         <v>412</v>
       </c>
@@ -15777,7 +15778,7 @@
       <c r="E88" s="122"/>
     </row>
     <row r="89" spans="1:5">
-      <c r="A89" s="145"/>
+      <c r="A89" s="156"/>
       <c r="B89" s="121" t="s">
         <v>413</v>
       </c>
@@ -15788,7 +15789,7 @@
       <c r="E89" s="122"/>
     </row>
     <row r="90" spans="1:5">
-      <c r="A90" s="145"/>
+      <c r="A90" s="156"/>
       <c r="B90" s="121" t="s">
         <v>414</v>
       </c>
@@ -15799,7 +15800,7 @@
       <c r="E90" s="122"/>
     </row>
     <row r="91" spans="1:5">
-      <c r="A91" s="145"/>
+      <c r="A91" s="156"/>
       <c r="B91" s="121" t="s">
         <v>415</v>
       </c>
@@ -15810,7 +15811,7 @@
       <c r="E91" s="122"/>
     </row>
     <row r="92" spans="1:5">
-      <c r="A92" s="145"/>
+      <c r="A92" s="156"/>
       <c r="B92" s="121" t="s">
         <v>416</v>
       </c>
@@ -15821,7 +15822,7 @@
       <c r="E92" s="122"/>
     </row>
     <row r="93" spans="1:5">
-      <c r="A93" s="145"/>
+      <c r="A93" s="156"/>
       <c r="B93" s="121" t="s">
         <v>418</v>
       </c>
@@ -15834,7 +15835,7 @@
       <c r="E93" s="122"/>
     </row>
     <row r="94" spans="1:5">
-      <c r="A94" s="145"/>
+      <c r="A94" s="156"/>
       <c r="B94" s="121" t="s">
         <v>421</v>
       </c>
@@ -15847,7 +15848,7 @@
       <c r="E94" s="122"/>
     </row>
     <row r="95" spans="1:5">
-      <c r="A95" s="145"/>
+      <c r="A95" s="156"/>
       <c r="B95" s="121" t="s">
         <v>424</v>
       </c>
@@ -15858,7 +15859,7 @@
       <c r="E95" s="122"/>
     </row>
     <row r="96" spans="1:5">
-      <c r="A96" s="145"/>
+      <c r="A96" s="156"/>
       <c r="B96" s="121" t="s">
         <v>426</v>
       </c>
@@ -15871,7 +15872,7 @@
       <c r="E96" s="122"/>
     </row>
     <row r="97" spans="1:5">
-      <c r="A97" s="145"/>
+      <c r="A97" s="156"/>
       <c r="B97" s="121" t="s">
         <v>429</v>
       </c>
@@ -15882,7 +15883,7 @@
       <c r="E97" s="122"/>
     </row>
     <row r="98" spans="1:5">
-      <c r="A98" s="145"/>
+      <c r="A98" s="156"/>
       <c r="B98" s="121" t="s">
         <v>431</v>
       </c>
@@ -15893,7 +15894,7 @@
       <c r="E98" s="122"/>
     </row>
     <row r="99" spans="1:5">
-      <c r="A99" s="145"/>
+      <c r="A99" s="156"/>
       <c r="B99" s="121" t="s">
         <v>433</v>
       </c>
@@ -15904,7 +15905,7 @@
       <c r="E99" s="122"/>
     </row>
     <row r="100" spans="1:5">
-      <c r="A100" s="145"/>
+      <c r="A100" s="156"/>
       <c r="B100" s="121" t="s">
         <v>434</v>
       </c>
@@ -15915,7 +15916,7 @@
       <c r="E100" s="122"/>
     </row>
     <row r="101" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A101" s="146"/>
+      <c r="A101" s="157"/>
       <c r="B101" s="121" t="s">
         <v>435</v>
       </c>
@@ -15937,7 +15938,7 @@
       <c r="E102" s="125"/>
     </row>
     <row r="103" spans="1:5">
-      <c r="A103" s="144" t="s">
+      <c r="A103" s="155" t="s">
         <v>179</v>
       </c>
       <c r="B103" s="119" t="s">
@@ -15950,7 +15951,7 @@
       <c r="E103" s="122"/>
     </row>
     <row r="104" spans="1:5" ht="17.25">
-      <c r="A104" s="145"/>
+      <c r="A104" s="156"/>
       <c r="B104" s="121" t="s">
         <v>441</v>
       </c>
@@ -15961,7 +15962,7 @@
       <c r="E104" s="122"/>
     </row>
     <row r="105" spans="1:5">
-      <c r="A105" s="145"/>
+      <c r="A105" s="156"/>
       <c r="B105" s="121" t="s">
         <v>443</v>
       </c>
@@ -15972,7 +15973,7 @@
       <c r="E105" s="122"/>
     </row>
     <row r="106" spans="1:5">
-      <c r="A106" s="145"/>
+      <c r="A106" s="156"/>
       <c r="B106" s="121" t="s">
         <v>445</v>
       </c>
@@ -15983,7 +15984,7 @@
       <c r="E106" s="122"/>
     </row>
     <row r="107" spans="1:5">
-      <c r="A107" s="145"/>
+      <c r="A107" s="156"/>
       <c r="B107" s="121" t="s">
         <v>447</v>
       </c>
@@ -15994,7 +15995,7 @@
       <c r="E107" s="122"/>
     </row>
     <row r="108" spans="1:5">
-      <c r="A108" s="145"/>
+      <c r="A108" s="156"/>
       <c r="B108" s="121" t="s">
         <v>449</v>
       </c>
@@ -16005,7 +16006,7 @@
       <c r="E108" s="122"/>
     </row>
     <row r="109" spans="1:5">
-      <c r="A109" s="145"/>
+      <c r="A109" s="156"/>
       <c r="B109" s="121" t="s">
         <v>451</v>
       </c>
@@ -16016,7 +16017,7 @@
       <c r="E109" s="122"/>
     </row>
     <row r="110" spans="1:5">
-      <c r="A110" s="145"/>
+      <c r="A110" s="156"/>
       <c r="B110" s="121" t="s">
         <v>453</v>
       </c>
@@ -16027,7 +16028,7 @@
       <c r="E110" s="122"/>
     </row>
     <row r="111" spans="1:5">
-      <c r="A111" s="145"/>
+      <c r="A111" s="156"/>
       <c r="B111" s="121" t="s">
         <v>455</v>
       </c>
@@ -16038,7 +16039,7 @@
       <c r="E111" s="122"/>
     </row>
     <row r="112" spans="1:5">
-      <c r="A112" s="145"/>
+      <c r="A112" s="156"/>
       <c r="B112" s="121" t="s">
         <v>457</v>
       </c>
@@ -16049,7 +16050,7 @@
       <c r="E112" s="122"/>
     </row>
     <row r="113" spans="1:5">
-      <c r="A113" s="145"/>
+      <c r="A113" s="156"/>
       <c r="B113" s="121" t="s">
         <v>459</v>
       </c>
@@ -16060,7 +16061,7 @@
       <c r="E113" s="122"/>
     </row>
     <row r="114" spans="1:5">
-      <c r="A114" s="145"/>
+      <c r="A114" s="156"/>
       <c r="B114" s="121" t="s">
         <v>461</v>
       </c>
@@ -16071,7 +16072,7 @@
       <c r="E114" s="122"/>
     </row>
     <row r="115" spans="1:5">
-      <c r="A115" s="145"/>
+      <c r="A115" s="156"/>
       <c r="B115" s="121" t="s">
         <v>463</v>
       </c>
@@ -16082,7 +16083,7 @@
       <c r="E115" s="122"/>
     </row>
     <row r="116" spans="1:5">
-      <c r="A116" s="145"/>
+      <c r="A116" s="156"/>
       <c r="B116" s="121" t="s">
         <v>465</v>
       </c>
@@ -16095,7 +16096,7 @@
       <c r="E116" s="122"/>
     </row>
     <row r="117" spans="1:5">
-      <c r="A117" s="145"/>
+      <c r="A117" s="156"/>
       <c r="B117" s="121" t="s">
         <v>468</v>
       </c>
@@ -16106,7 +16107,7 @@
       <c r="E117" s="122"/>
     </row>
     <row r="118" spans="1:5">
-      <c r="A118" s="145"/>
+      <c r="A118" s="156"/>
       <c r="B118" s="121" t="s">
         <v>470</v>
       </c>
@@ -16117,7 +16118,7 @@
       <c r="E118" s="122"/>
     </row>
     <row r="119" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A119" s="146"/>
+      <c r="A119" s="157"/>
       <c r="B119" s="127" t="s">
         <v>472</v>
       </c>
@@ -16165,28 +16166,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="147"/>
-      <c r="B1" s="147"/>
-      <c r="C1" s="147"/>
-      <c r="D1" s="147"/>
+      <c r="A1" s="129"/>
+      <c r="B1" s="129"/>
+      <c r="C1" s="129"/>
+      <c r="D1" s="129"/>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="147"/>
-      <c r="B2" s="147"/>
-      <c r="C2" s="147"/>
-      <c r="D2" s="147"/>
+      <c r="A2" s="129"/>
+      <c r="B2" s="129"/>
+      <c r="C2" s="129"/>
+      <c r="D2" s="129"/>
     </row>
     <row r="3" spans="1:4" ht="15.75">
-      <c r="A3" s="151" t="s">
+      <c r="A3" s="132" t="s">
         <v>474</v>
       </c>
-      <c r="B3" s="151" t="s">
+      <c r="B3" s="132" t="s">
         <v>475</v>
       </c>
-      <c r="C3" s="151" t="s">
+      <c r="C3" s="132" t="s">
         <v>476</v>
       </c>
-      <c r="D3" s="151" t="s">
+      <c r="D3" s="132" t="s">
         <v>477</v>
       </c>
     </row>
@@ -16194,97 +16195,97 @@
       <c r="A4" s="162" t="s">
         <v>478</v>
       </c>
-      <c r="B4" s="152" t="s">
+      <c r="B4" s="133" t="s">
         <v>479</v>
       </c>
-      <c r="C4" s="152" t="s">
+      <c r="C4" s="133" t="s">
         <v>480</v>
       </c>
-      <c r="D4" s="152" t="s">
+      <c r="D4" s="133" t="s">
         <v>481</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="163"/>
-      <c r="B5" s="152" t="s">
+      <c r="B5" s="133" t="s">
         <v>482</v>
       </c>
-      <c r="C5" s="152" t="s">
+      <c r="C5" s="133" t="s">
         <v>483</v>
       </c>
-      <c r="D5" s="152" t="s">
+      <c r="D5" s="133" t="s">
         <v>484</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="163"/>
-      <c r="B6" s="152" t="s">
+      <c r="B6" s="133" t="s">
         <v>485</v>
       </c>
-      <c r="C6" s="152" t="s">
+      <c r="C6" s="133" t="s">
         <v>486</v>
       </c>
-      <c r="D6" s="152" t="s">
+      <c r="D6" s="133" t="s">
         <v>487</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="163"/>
-      <c r="B7" s="152" t="s">
+      <c r="B7" s="133" t="s">
         <v>488</v>
       </c>
-      <c r="C7" s="152" t="s">
+      <c r="C7" s="133" t="s">
         <v>489</v>
       </c>
-      <c r="D7" s="152" t="s">
+      <c r="D7" s="133" t="s">
         <v>490</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="163"/>
-      <c r="B8" s="152" t="s">
+      <c r="B8" s="133" t="s">
         <v>491</v>
       </c>
-      <c r="C8" s="152" t="s">
+      <c r="C8" s="133" t="s">
         <v>492</v>
       </c>
-      <c r="D8" s="152" t="s">
+      <c r="D8" s="133" t="s">
         <v>493</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="163"/>
-      <c r="B9" s="152" t="s">
+      <c r="B9" s="133" t="s">
         <v>494</v>
       </c>
-      <c r="C9" s="152" t="s">
+      <c r="C9" s="133" t="s">
         <v>495</v>
       </c>
-      <c r="D9" s="152" t="s">
+      <c r="D9" s="133" t="s">
         <v>496</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="163"/>
-      <c r="B10" s="152" t="s">
+      <c r="B10" s="133" t="s">
         <v>497</v>
       </c>
-      <c r="C10" s="152" t="s">
+      <c r="C10" s="133" t="s">
         <v>498</v>
       </c>
-      <c r="D10" s="152" t="s">
+      <c r="D10" s="133" t="s">
         <v>499</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="164"/>
-      <c r="B11" s="152" t="s">
+      <c r="B11" s="133" t="s">
         <v>500</v>
       </c>
-      <c r="C11" s="152" t="s">
+      <c r="C11" s="133" t="s">
         <v>501</v>
       </c>
-      <c r="D11" s="152" t="s">
+      <c r="D11" s="133" t="s">
         <v>502</v>
       </c>
     </row>
@@ -16292,49 +16293,49 @@
       <c r="A12" s="165" t="s">
         <v>503</v>
       </c>
-      <c r="B12" s="153" t="s">
+      <c r="B12" s="134" t="s">
         <v>504</v>
       </c>
-      <c r="C12" s="153" t="s">
+      <c r="C12" s="134" t="s">
         <v>505</v>
       </c>
-      <c r="D12" s="153" t="s">
+      <c r="D12" s="134" t="s">
         <v>506</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="166"/>
-      <c r="B13" s="153" t="s">
+      <c r="B13" s="134" t="s">
         <v>507</v>
       </c>
-      <c r="C13" s="153" t="s">
+      <c r="C13" s="134" t="s">
         <v>508</v>
       </c>
-      <c r="D13" s="153" t="s">
+      <c r="D13" s="134" t="s">
         <v>509</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="166"/>
-      <c r="B14" s="153" t="s">
+      <c r="B14" s="134" t="s">
         <v>510</v>
       </c>
-      <c r="C14" s="153" t="s">
+      <c r="C14" s="134" t="s">
         <v>511</v>
       </c>
-      <c r="D14" s="153" t="s">
+      <c r="D14" s="134" t="s">
         <v>512</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="167"/>
-      <c r="B15" s="153" t="s">
+      <c r="B15" s="134" t="s">
         <v>513</v>
       </c>
-      <c r="C15" s="153" t="s">
+      <c r="C15" s="134" t="s">
         <v>514</v>
       </c>
-      <c r="D15" s="153" t="s">
+      <c r="D15" s="134" t="s">
         <v>515</v>
       </c>
     </row>
@@ -16354,7 +16355,7 @@
   </sheetPr>
   <dimension ref="A3:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4:E4"/>
     </sheetView>
   </sheetViews>
@@ -16368,120 +16369,120 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:5" ht="15.75">
-      <c r="A3" s="154" t="s">
+      <c r="A3" s="135" t="s">
         <v>516</v>
       </c>
-      <c r="B3" s="154" t="s">
+      <c r="B3" s="135" t="s">
         <v>517</v>
       </c>
-      <c r="C3" s="154" t="s">
+      <c r="C3" s="135" t="s">
         <v>518</v>
       </c>
-      <c r="D3" s="155" t="s">
+      <c r="D3" s="158" t="s">
         <v>519</v>
       </c>
-      <c r="E3" s="156"/>
+      <c r="E3" s="159"/>
     </row>
     <row r="4" spans="1:5" ht="83.25" customHeight="1">
-      <c r="A4" s="157">
+      <c r="A4" s="136">
         <v>45021</v>
       </c>
-      <c r="B4" s="158" t="s">
+      <c r="B4" s="137" t="s">
         <v>520</v>
       </c>
-      <c r="C4" s="159" t="s">
+      <c r="C4" s="138" t="s">
         <v>521</v>
       </c>
-      <c r="D4" s="160" t="s">
+      <c r="D4" s="139" t="s">
         <v>522</v>
       </c>
-      <c r="E4" s="160" t="s">
+      <c r="E4" s="139" t="s">
         <v>523</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="150"/>
+      <c r="A5" s="131"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="150"/>
+      <c r="A6" s="131"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="150"/>
+      <c r="A7" s="131"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="150"/>
+      <c r="A8" s="131"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="150"/>
+      <c r="A9" s="131"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="150"/>
+      <c r="A10" s="131"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="150"/>
+      <c r="A11" s="131"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="150"/>
+      <c r="A12" s="131"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="150"/>
+      <c r="A13" s="131"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="150"/>
+      <c r="A14" s="131"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="150"/>
+      <c r="A15" s="131"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="150"/>
+      <c r="A16" s="131"/>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" s="150"/>
+      <c r="A17" s="131"/>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18" s="150"/>
+      <c r="A18" s="131"/>
     </row>
     <row r="19" spans="1:1">
-      <c r="A19" s="150"/>
+      <c r="A19" s="131"/>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" s="150"/>
+      <c r="A20" s="131"/>
     </row>
     <row r="21" spans="1:1">
-      <c r="A21" s="150"/>
+      <c r="A21" s="131"/>
     </row>
     <row r="22" spans="1:1">
-      <c r="A22" s="150"/>
+      <c r="A22" s="131"/>
     </row>
     <row r="23" spans="1:1">
-      <c r="A23" s="150"/>
+      <c r="A23" s="131"/>
     </row>
     <row r="24" spans="1:1">
-      <c r="A24" s="150"/>
+      <c r="A24" s="131"/>
     </row>
     <row r="25" spans="1:1">
-      <c r="A25" s="150"/>
+      <c r="A25" s="131"/>
     </row>
     <row r="26" spans="1:1">
-      <c r="A26" s="150"/>
+      <c r="A26" s="131"/>
     </row>
     <row r="27" spans="1:1">
-      <c r="A27" s="150"/>
+      <c r="A27" s="131"/>
     </row>
     <row r="28" spans="1:1">
-      <c r="A28" s="150"/>
+      <c r="A28" s="131"/>
     </row>
     <row r="29" spans="1:1">
-      <c r="A29" s="150"/>
+      <c r="A29" s="131"/>
     </row>
     <row r="30" spans="1:1">
-      <c r="A30" s="150"/>
+      <c r="A30" s="131"/>
     </row>
     <row r="31" spans="1:1">
-      <c r="A31" s="150"/>
+      <c r="A31" s="131"/>
     </row>
     <row r="32" spans="1:1">
-      <c r="A32" s="150"/>
+      <c r="A32" s="131"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>